<commit_message>
Add GSW vs HOU GM6/7 & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_playoffs_stats.xlsx
+++ b/data/gsw_box_score_team_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1620,6 +1620,422 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>35</v>
+      </c>
+      <c r="H12" t="n">
+        <v>78</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.449</v>
+      </c>
+      <c r="J12" t="n">
+        <v>12</v>
+      </c>
+      <c r="K12" t="n">
+        <v>30</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M12" t="n">
+        <v>33</v>
+      </c>
+      <c r="N12" t="n">
+        <v>46</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.717</v>
+      </c>
+      <c r="P12" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>35</v>
+      </c>
+      <c r="R12" t="n">
+        <v>46</v>
+      </c>
+      <c r="S12" t="n">
+        <v>23</v>
+      </c>
+      <c r="T12" t="n">
+        <v>12</v>
+      </c>
+      <c r="U12" t="n">
+        <v>5</v>
+      </c>
+      <c r="V12" t="n">
+        <v>11</v>
+      </c>
+      <c r="W12" t="n">
+        <v>18</v>
+      </c>
+      <c r="X12" t="n">
+        <v>115</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>37</v>
+      </c>
+      <c r="H13" t="n">
+        <v>90</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.411</v>
+      </c>
+      <c r="J13" t="n">
+        <v>15</v>
+      </c>
+      <c r="K13" t="n">
+        <v>49</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.306</v>
+      </c>
+      <c r="M13" t="n">
+        <v>18</v>
+      </c>
+      <c r="N13" t="n">
+        <v>22</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="P13" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>29</v>
+      </c>
+      <c r="R13" t="n">
+        <v>42</v>
+      </c>
+      <c r="S13" t="n">
+        <v>26</v>
+      </c>
+      <c r="T13" t="n">
+        <v>6</v>
+      </c>
+      <c r="U13" t="n">
+        <v>6</v>
+      </c>
+      <c r="V13" t="n">
+        <v>16</v>
+      </c>
+      <c r="W13" t="n">
+        <v>30</v>
+      </c>
+      <c r="X13" t="n">
+        <v>107</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>-8</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>39</v>
+      </c>
+      <c r="H14" t="n">
+        <v>82</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="J14" t="n">
+        <v>18</v>
+      </c>
+      <c r="K14" t="n">
+        <v>43</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.419</v>
+      </c>
+      <c r="M14" t="n">
+        <v>7</v>
+      </c>
+      <c r="N14" t="n">
+        <v>9</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="P14" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>35</v>
+      </c>
+      <c r="R14" t="n">
+        <v>38</v>
+      </c>
+      <c r="S14" t="n">
+        <v>24</v>
+      </c>
+      <c r="T14" t="n">
+        <v>6</v>
+      </c>
+      <c r="U14" t="n">
+        <v>8</v>
+      </c>
+      <c r="V14" t="n">
+        <v>7</v>
+      </c>
+      <c r="W14" t="n">
+        <v>14</v>
+      </c>
+      <c r="X14" t="n">
+        <v>103</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>34</v>
+      </c>
+      <c r="H15" t="n">
+        <v>84</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.405</v>
+      </c>
+      <c r="J15" t="n">
+        <v>6</v>
+      </c>
+      <c r="K15" t="n">
+        <v>18</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="M15" t="n">
+        <v>15</v>
+      </c>
+      <c r="N15" t="n">
+        <v>21</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="P15" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>38</v>
+      </c>
+      <c r="R15" t="n">
+        <v>52</v>
+      </c>
+      <c r="S15" t="n">
+        <v>14</v>
+      </c>
+      <c r="T15" t="n">
+        <v>5</v>
+      </c>
+      <c r="U15" t="n">
+        <v>5</v>
+      </c>
+      <c r="V15" t="n">
+        <v>11</v>
+      </c>
+      <c r="W15" t="n">
+        <v>14</v>
+      </c>
+      <c r="X15" t="n">
+        <v>89</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>-14</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>